<commit_message>
Update cleaning with species level cleaning
</commit_message>
<xml_diff>
--- a/R/2017_10_06_Compiled_LN2_Shallow (0m to 120m)_newcleaned.xlsx
+++ b/R/2017_10_06_Compiled_LN2_Shallow (0m to 120m)_newcleaned.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeozy\Documents\Yale-NUS\Y3S1\UROPS\Data\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TMSI-REL\Desktop\Zhi Yi's Working Folder\UROPS\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BEBF598-5F91-4CC5-96ED-BB39DE38A1B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240FE94D-928C-4C3A-AFCF-3DC2665457FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25599" windowHeight="15995" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15990" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
     <sheet name="LN2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3702,10 +3707,10 @@
       <selection sqref="A1:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="16.100000000000001"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.453125" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3922,9 +3927,9 @@
       <selection sqref="A1:B821"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="16.100000000000001"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8934,17 +8939,17 @@
   <dimension ref="A1:T398"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A378" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K395" sqref="K395"/>
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M153" sqref="M153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="16.100000000000001"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="17.7265625" style="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.90625" style="42" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="11" max="11" width="17.75" style="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.875" style="42" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">

</xml_diff>